<commit_message>
Updated to include a vertical menu, placeholder-image-logo on menu, profiles updated. Updated publishing script to account for name variations.
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Emily_Smenderovac/Author_form.xlsx
+++ b/website_content_creation/authors/Emily_Smenderovac/Author_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\Emily_Smenderovac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\authors\Emily_Smenderovac\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">Trained in microbial ecology and bioinformatic analysis of community datasets. </t>
   </si>
   <si>
-    <t>I completed my M.Sc. Forestry studying microbial community structures in coarse woody residues and harvesting impacted soils from sites in Ontario, Canada.  I enjoy R coding, troubleshooting and teaching, lab work and field work.</t>
-  </si>
-  <si>
     <t>WETlab Contributors from the GLFC</t>
+  </si>
+  <si>
+    <t>I completed my M.Sc. Forestry studying microbial community structures in coarse woody residues and harvesting impacted soils from sites in Ontario, Canada.  I enjoy R coding, troubleshooting and teaching, lab work and, field work.</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +786,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>